<commit_message>
Get fimat a table
</commit_message>
<xml_diff>
--- a/salida.xlsx
+++ b/salida.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,14 +27,20 @@
     </font>
     <font>
       <name val="Eras Medium ITC"/>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <sz val="16"/>
     </font>
     <font>
       <name val="Eras Medium ITC"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Eras Medium ITC"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Eras Medium ITC"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -45,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -54,18 +60,135 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thick"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thick"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thick"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thick"/>
+      <top style="medium"/>
+      <bottom style="thick"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -441,13 +564,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="3.8" customWidth="1" min="1" max="1"/>
-    <col width="2.8" customWidth="1" min="2" max="2"/>
-    <col width="13.8" customWidth="1" min="3" max="3"/>
-    <col width="18.8" customWidth="1" min="4" max="4"/>
-    <col width="1.8" customWidth="1" min="5" max="5"/>
-    <col width="18.8" customWidth="1" min="6" max="6"/>
-    <col width="18.8" customWidth="1" min="7" max="7"/>
+    <col width="5" customWidth="1" min="1" max="1"/>
+    <col width="5" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="3" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,194 +579,222 @@
           <t>CUADRO DE CONSTRUCCION</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+      <c r="G1" s="4" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>LADO</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="B2" s="6" t="n"/>
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>RUMBO</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>DISTANCIA</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" s="7" t="inlineStr">
         <is>
           <t>CORDENADAS</t>
         </is>
       </c>
-      <c r="G2" s="1" t="n"/>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>EST</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B3" s="10" t="inlineStr">
         <is>
           <t>PV</t>
         </is>
       </c>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="C3" s="11" t="n"/>
+      <c r="D3" s="10" t="n"/>
+      <c r="E3" s="10" t="n"/>
+      <c r="F3" s="10" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
+      <c r="G3" s="12" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr"/>
-      <c r="B4" s="1" t="inlineStr"/>
-      <c r="C4" s="1" t="inlineStr"/>
-      <c r="D4" s="1" t="inlineStr"/>
-      <c r="E4" s="1" t="n">
+      <c r="A4" s="13" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr"/>
+      <c r="C4" s="6" t="inlineStr"/>
+      <c r="D4" s="7" t="inlineStr"/>
+      <c r="E4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>452515.2088625222</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>2130778.89036045</v>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>452,515.2089</t>
+        </is>
+      </c>
+      <c r="G4" s="8" t="inlineStr">
+        <is>
+          <t>2,130,778.8904</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>N 5.69508° E</t>
         </is>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>9.400000000022892</v>
-      </c>
-      <c r="E5" s="1" t="n">
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>9.400</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>452515.2088625222</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>2130778.89036045</v>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>452,515.2089</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>2,130,778.8904</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>N 85.67346° W</t>
         </is>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>62.24243401145041</v>
-      </c>
-      <c r="E6" s="1" t="n">
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>62.242</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>452516.1416657649</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>2130788.243962863</v>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>452,516.1417</t>
+        </is>
+      </c>
+      <c r="G6" s="12" t="inlineStr">
+        <is>
+          <t>2,130,788.2440</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>S 3.03921° W</t>
         </is>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>8.899999999902336</v>
-      </c>
-      <c r="E7" s="1" t="n">
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>8.900</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>452454.0766039148</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>2130792.939566043</v>
+      <c r="F7" s="10" t="inlineStr">
+        <is>
+          <t>452,454.0766</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>2,130,792.9396</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="inlineStr">
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>S 85.21045° E</t>
         </is>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>61.82000000001754</v>
-      </c>
-      <c r="E8" s="1" t="n">
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>61.820</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>452453.6047310909</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>2130784.052084058</v>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>452,453.6047</t>
+        </is>
+      </c>
+      <c r="G8" s="12" t="inlineStr">
+        <is>
+          <t>2,130,784.0521</t>
+        </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>SUPERFICIE 567.4266967773438</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
-      <c r="E9" s="1" t="n"/>
-      <c r="F9" s="1" t="n"/>
-      <c r="G9" s="1" t="n"/>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="15" t="inlineStr">
+        <is>
+          <t>SUPERFICIE 567.427 m2</t>
+        </is>
+      </c>
+      <c r="B9" s="16" t="n"/>
+      <c r="C9" s="16" t="n"/>
+      <c r="D9" s="17" t="n"/>
+      <c r="E9" s="17" t="n"/>
+      <c r="F9" s="17" t="n"/>
+      <c r="G9" s="18" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>